<commit_message>
Add Whiteley et al., to reference models
</commit_message>
<xml_diff>
--- a/amnh/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
+++ b/amnh/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\amnh\datasets\MigratoryModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2ED6CD-102D-411E-8F0F-1ACC634187BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C16C28-1970-4728-83AB-3EBD17864561}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
   </bookViews>
   <sheets>
     <sheet name="MigratoryModel_TableauData" sheetId="1" r:id="rId1"/>
     <sheet name="ZoneCenterLocations" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MigratoryModel_TableauData!$A$1:$J$171</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MigratoryModel_TableauData!$A$1:$J$265</definedName>
   </definedNames>
   <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="89">
   <si>
     <t>A</t>
   </si>
@@ -281,6 +281,21 @@
   </si>
   <si>
     <t>Combined</t>
+  </si>
+  <si>
+    <t>K-S</t>
+  </si>
+  <si>
+    <t>L-D</t>
+  </si>
+  <si>
+    <t>M-R</t>
+  </si>
+  <si>
+    <t>K-N</t>
+  </si>
+  <si>
+    <t>Whiteley et al., 2018</t>
   </si>
 </sst>
 </file>
@@ -632,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7D369B-DF5B-472F-B73D-7CCA41A92755}">
-  <dimension ref="A1:J231"/>
+  <dimension ref="A1:J265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="M222" sqref="M222"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="G221" sqref="G221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7624,8 +7639,892 @@
         <v>1</v>
       </c>
     </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>54</v>
+      </c>
+      <c r="B232">
+        <v>1</v>
+      </c>
+      <c r="D232">
+        <v>2.3488888888888888</v>
+      </c>
+      <c r="E232">
+        <v>10.31111111111111</v>
+      </c>
+      <c r="F232" t="s">
+        <v>0</v>
+      </c>
+      <c r="H232" t="s">
+        <v>88</v>
+      </c>
+      <c r="I232" t="s">
+        <v>76</v>
+      </c>
+      <c r="J232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>54</v>
+      </c>
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="D233">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E233">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F233" t="s">
+        <v>2</v>
+      </c>
+      <c r="H233" t="s">
+        <v>88</v>
+      </c>
+      <c r="I233" t="s">
+        <v>76</v>
+      </c>
+      <c r="J233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>55</v>
+      </c>
+      <c r="B234">
+        <v>1</v>
+      </c>
+      <c r="D234">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E234">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F234" t="s">
+        <v>2</v>
+      </c>
+      <c r="H234" t="s">
+        <v>88</v>
+      </c>
+      <c r="I234" t="s">
+        <v>76</v>
+      </c>
+      <c r="J234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>55</v>
+      </c>
+      <c r="B235">
+        <v>2</v>
+      </c>
+      <c r="D235">
+        <v>-1.753125</v>
+      </c>
+      <c r="E235">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F235" t="s">
+        <v>1</v>
+      </c>
+      <c r="H235" t="s">
+        <v>88</v>
+      </c>
+      <c r="I235" t="s">
+        <v>76</v>
+      </c>
+      <c r="J235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>21</v>
+      </c>
+      <c r="B236">
+        <v>1</v>
+      </c>
+      <c r="D236">
+        <v>-0.40769230769230752</v>
+      </c>
+      <c r="E236">
+        <v>21.388461538461538</v>
+      </c>
+      <c r="F236" t="s">
+        <v>2</v>
+      </c>
+      <c r="H236" t="s">
+        <v>88</v>
+      </c>
+      <c r="I236" t="s">
+        <v>76</v>
+      </c>
+      <c r="J236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>21</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+      <c r="D237">
+        <v>-1.78</v>
+      </c>
+      <c r="E237">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F237" t="s">
+        <v>3</v>
+      </c>
+      <c r="H237" t="s">
+        <v>88</v>
+      </c>
+      <c r="I237" t="s">
+        <v>76</v>
+      </c>
+      <c r="J237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>19</v>
+      </c>
+      <c r="B238">
+        <v>1</v>
+      </c>
+      <c r="D238">
+        <v>-1.753125</v>
+      </c>
+      <c r="E238">
+        <v>13.153124999999999</v>
+      </c>
+      <c r="F238" t="s">
+        <v>1</v>
+      </c>
+      <c r="H238" t="s">
+        <v>88</v>
+      </c>
+      <c r="I238" t="s">
+        <v>76</v>
+      </c>
+      <c r="J238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>19</v>
+      </c>
+      <c r="B239">
+        <v>2</v>
+      </c>
+      <c r="D239">
+        <v>-5.5714285714285703</v>
+      </c>
+      <c r="E239">
+        <v>15.75</v>
+      </c>
+      <c r="F239" t="s">
+        <v>7</v>
+      </c>
+      <c r="H239" t="s">
+        <v>88</v>
+      </c>
+      <c r="I239" t="s">
+        <v>76</v>
+      </c>
+      <c r="J239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>63</v>
+      </c>
+      <c r="B240">
+        <v>1</v>
+      </c>
+      <c r="D240">
+        <v>-5.5714285714285703</v>
+      </c>
+      <c r="E240">
+        <v>15.75</v>
+      </c>
+      <c r="F240" t="s">
+        <v>7</v>
+      </c>
+      <c r="H240" t="s">
+        <v>88</v>
+      </c>
+      <c r="I240" t="s">
+        <v>76</v>
+      </c>
+      <c r="J240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>63</v>
+      </c>
+      <c r="B241">
+        <v>2</v>
+      </c>
+      <c r="D241">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E241">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F241" t="s">
+        <v>9</v>
+      </c>
+      <c r="H241" t="s">
+        <v>88</v>
+      </c>
+      <c r="I241" t="s">
+        <v>76</v>
+      </c>
+      <c r="J241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>84</v>
+      </c>
+      <c r="B242">
+        <v>1</v>
+      </c>
+      <c r="D242">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E242">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F242" t="s">
+        <v>9</v>
+      </c>
+      <c r="H242" t="s">
+        <v>88</v>
+      </c>
+      <c r="I242" t="s">
+        <v>76</v>
+      </c>
+      <c r="J242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>84</v>
+      </c>
+      <c r="B243">
+        <v>2</v>
+      </c>
+      <c r="D243">
+        <v>-23.125</v>
+      </c>
+      <c r="E243">
+        <v>29.665624999999999</v>
+      </c>
+      <c r="F243" t="s">
+        <v>15</v>
+      </c>
+      <c r="H243" t="s">
+        <v>88</v>
+      </c>
+      <c r="I243" t="s">
+        <v>76</v>
+      </c>
+      <c r="J243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>64</v>
+      </c>
+      <c r="B244">
+        <v>1</v>
+      </c>
+      <c r="D244">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E244">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F244" t="s">
+        <v>9</v>
+      </c>
+      <c r="H244" t="s">
+        <v>88</v>
+      </c>
+      <c r="I244" t="s">
+        <v>76</v>
+      </c>
+      <c r="J244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>64</v>
+      </c>
+      <c r="B245">
+        <v>2</v>
+      </c>
+      <c r="D245">
+        <v>-9.16</v>
+      </c>
+      <c r="E245">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F245" t="s">
+        <v>10</v>
+      </c>
+      <c r="H245" t="s">
+        <v>88</v>
+      </c>
+      <c r="I245" t="s">
+        <v>76</v>
+      </c>
+      <c r="J245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>85</v>
+      </c>
+      <c r="B246">
+        <v>1</v>
+      </c>
+      <c r="D246">
+        <v>-9.16</v>
+      </c>
+      <c r="E246">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F246" t="s">
+        <v>10</v>
+      </c>
+      <c r="H246" t="s">
+        <v>88</v>
+      </c>
+      <c r="I246" t="s">
+        <v>76</v>
+      </c>
+      <c r="J246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>85</v>
+      </c>
+      <c r="B247">
+        <v>2</v>
+      </c>
+      <c r="D247">
+        <v>-1.78</v>
+      </c>
+      <c r="E247">
+        <v>27.603999999999996</v>
+      </c>
+      <c r="F247" t="s">
+        <v>3</v>
+      </c>
+      <c r="H247" t="s">
+        <v>88</v>
+      </c>
+      <c r="I247" t="s">
+        <v>76</v>
+      </c>
+      <c r="J247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>29</v>
+      </c>
+      <c r="B248">
+        <v>1</v>
+      </c>
+      <c r="D248">
+        <v>-9.16</v>
+      </c>
+      <c r="E248">
+        <v>26.439999999999998</v>
+      </c>
+      <c r="F248" t="s">
+        <v>10</v>
+      </c>
+      <c r="H248" t="s">
+        <v>88</v>
+      </c>
+      <c r="I248" t="s">
+        <v>76</v>
+      </c>
+      <c r="J248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>29</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="D249">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E249">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F249" t="s">
+        <v>11</v>
+      </c>
+      <c r="H249" t="s">
+        <v>88</v>
+      </c>
+      <c r="I249" t="s">
+        <v>76</v>
+      </c>
+      <c r="J249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>51</v>
+      </c>
+      <c r="B250">
+        <v>1</v>
+      </c>
+      <c r="D250">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E250">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F250" t="s">
+        <v>11</v>
+      </c>
+      <c r="H250" t="s">
+        <v>88</v>
+      </c>
+      <c r="I250" t="s">
+        <v>76</v>
+      </c>
+      <c r="J250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>51</v>
+      </c>
+      <c r="B251">
+        <v>2</v>
+      </c>
+      <c r="D251">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E251">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F251" t="s">
+        <v>8</v>
+      </c>
+      <c r="H251" t="s">
+        <v>88</v>
+      </c>
+      <c r="I251" t="s">
+        <v>76</v>
+      </c>
+      <c r="J251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>58</v>
+      </c>
+      <c r="B252">
+        <v>1</v>
+      </c>
+      <c r="D252">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E252">
+        <v>33</v>
+      </c>
+      <c r="F252" t="s">
+        <v>5</v>
+      </c>
+      <c r="H252" t="s">
+        <v>88</v>
+      </c>
+      <c r="I252" t="s">
+        <v>76</v>
+      </c>
+      <c r="J252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>58</v>
+      </c>
+      <c r="B253">
+        <v>2</v>
+      </c>
+      <c r="D253">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E253">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F253" t="s">
+        <v>8</v>
+      </c>
+      <c r="H253" t="s">
+        <v>88</v>
+      </c>
+      <c r="I253" t="s">
+        <v>76</v>
+      </c>
+      <c r="J253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>86</v>
+      </c>
+      <c r="B254">
+        <v>1</v>
+      </c>
+      <c r="D254">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E254">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F254" t="s">
+        <v>11</v>
+      </c>
+      <c r="H254" t="s">
+        <v>88</v>
+      </c>
+      <c r="I254" t="s">
+        <v>76</v>
+      </c>
+      <c r="J254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>86</v>
+      </c>
+      <c r="B255">
+        <v>2</v>
+      </c>
+      <c r="D255">
+        <v>-15.824999999999999</v>
+      </c>
+      <c r="E255">
+        <v>15.45</v>
+      </c>
+      <c r="F255" t="s">
+        <v>14</v>
+      </c>
+      <c r="H255" t="s">
+        <v>88</v>
+      </c>
+      <c r="I255" t="s">
+        <v>76</v>
+      </c>
+      <c r="J255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>52</v>
+      </c>
+      <c r="B256">
+        <v>1</v>
+      </c>
+      <c r="D256">
+        <v>-13.122222222222224</v>
+      </c>
+      <c r="E256">
+        <v>29.1944444444444</v>
+      </c>
+      <c r="F256" t="s">
+        <v>11</v>
+      </c>
+      <c r="H256" t="s">
+        <v>88</v>
+      </c>
+      <c r="I256" t="s">
+        <v>76</v>
+      </c>
+      <c r="J256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>52</v>
+      </c>
+      <c r="B257">
+        <v>2</v>
+      </c>
+      <c r="D257">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E257">
+        <v>33</v>
+      </c>
+      <c r="F257" t="s">
+        <v>5</v>
+      </c>
+      <c r="H257" t="s">
+        <v>88</v>
+      </c>
+      <c r="I257" t="s">
+        <v>76</v>
+      </c>
+      <c r="J257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>58</v>
+      </c>
+      <c r="B258">
+        <v>1</v>
+      </c>
+      <c r="D258">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E258">
+        <v>33</v>
+      </c>
+      <c r="F258" t="s">
+        <v>5</v>
+      </c>
+      <c r="H258" t="s">
+        <v>88</v>
+      </c>
+      <c r="I258" t="s">
+        <v>76</v>
+      </c>
+      <c r="J258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>58</v>
+      </c>
+      <c r="B259">
+        <v>2</v>
+      </c>
+      <c r="D259">
+        <v>-1.44444444444444</v>
+      </c>
+      <c r="E259">
+        <v>30.911111111111115</v>
+      </c>
+      <c r="F259" t="s">
+        <v>8</v>
+      </c>
+      <c r="H259" t="s">
+        <v>88</v>
+      </c>
+      <c r="I259" t="s">
+        <v>76</v>
+      </c>
+      <c r="J259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>60</v>
+      </c>
+      <c r="B260">
+        <v>1</v>
+      </c>
+      <c r="D260">
+        <v>-3.7333333333333329</v>
+      </c>
+      <c r="E260">
+        <v>33</v>
+      </c>
+      <c r="F260" t="s">
+        <v>5</v>
+      </c>
+      <c r="H260" t="s">
+        <v>88</v>
+      </c>
+      <c r="I260" t="s">
+        <v>76</v>
+      </c>
+      <c r="J260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>60</v>
+      </c>
+      <c r="B261">
+        <v>2</v>
+      </c>
+      <c r="D261">
+        <v>-2.35</v>
+      </c>
+      <c r="E261">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F261" t="s">
+        <v>4</v>
+      </c>
+      <c r="H261" t="s">
+        <v>88</v>
+      </c>
+      <c r="I261" t="s">
+        <v>76</v>
+      </c>
+      <c r="J261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>70</v>
+      </c>
+      <c r="B262">
+        <v>1</v>
+      </c>
+      <c r="D262">
+        <v>-2.35</v>
+      </c>
+      <c r="E262">
+        <v>38.449999999999996</v>
+      </c>
+      <c r="F262" t="s">
+        <v>4</v>
+      </c>
+      <c r="H262" t="s">
+        <v>88</v>
+      </c>
+      <c r="I262" t="s">
+        <v>76</v>
+      </c>
+      <c r="J262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>70</v>
+      </c>
+      <c r="B263">
+        <v>2</v>
+      </c>
+      <c r="D263">
+        <v>-5.85</v>
+      </c>
+      <c r="E263">
+        <v>37.712499999999999</v>
+      </c>
+      <c r="F263" t="s">
+        <v>6</v>
+      </c>
+      <c r="H263" t="s">
+        <v>88</v>
+      </c>
+      <c r="I263" t="s">
+        <v>76</v>
+      </c>
+      <c r="J263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>87</v>
+      </c>
+      <c r="B264">
+        <v>1</v>
+      </c>
+      <c r="D264">
+        <v>-12.962999999999999</v>
+      </c>
+      <c r="E264">
+        <v>22.224999999999998</v>
+      </c>
+      <c r="F264" t="s">
+        <v>9</v>
+      </c>
+      <c r="H264" t="s">
+        <v>88</v>
+      </c>
+      <c r="I264" t="s">
+        <v>76</v>
+      </c>
+      <c r="J264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>87</v>
+      </c>
+      <c r="B265">
+        <v>2</v>
+      </c>
+      <c r="D265">
+        <v>-13.557142857142859</v>
+      </c>
+      <c r="E265">
+        <v>33.514285714285712</v>
+      </c>
+      <c r="F265" t="s">
+        <v>12</v>
+      </c>
+      <c r="H265" t="s">
+        <v>88</v>
+      </c>
+      <c r="I265" t="s">
+        <v>76</v>
+      </c>
+      <c r="J265">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J231" xr:uid="{303E4824-0DA0-4156-A165-CC92066081A2}"/>
+  <autoFilter ref="A1:J265" xr:uid="{303E4824-0DA0-4156-A165-CC92066081A2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add updated Whiteley coordinates to map
</commit_message>
<xml_diff>
--- a/amnh/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
+++ b/amnh/datasets/MigratoryModel/CombinedMigratoryModel_GuthrieZone_Path - AllModels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\BantuMigration\Github\amnh\datasets\MigratoryModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A85EB19-532B-470A-9C0C-DC4FF84E0ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35EF966-40DD-4218-996B-020DD9962364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48220AAF-5FA7-46D3-8056-2130CE6EF7AB}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="169">
   <si>
     <t>A</t>
   </si>
@@ -894,11 +894,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7D369B-DF5B-472F-B73D-7CCA41A92755}">
-  <dimension ref="A1:J401"/>
+  <dimension ref="A1:J403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A342" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A386" sqref="A386"/>
+      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C358" sqref="C358:C403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11199,6 +11199,12 @@
       <c r="B358">
         <v>1</v>
       </c>
+      <c r="D358">
+        <v>5.1657630000000001</v>
+      </c>
+      <c r="E358">
+        <v>10.159295</v>
+      </c>
       <c r="F358" s="1" t="s">
         <v>114</v>
       </c>
@@ -11219,6 +11225,12 @@
       <c r="B359">
         <v>2</v>
       </c>
+      <c r="D359">
+        <v>-0.64393199999999995</v>
+      </c>
+      <c r="E359">
+        <v>16.296029000000001</v>
+      </c>
       <c r="F359" s="1" t="s">
         <v>115</v>
       </c>
@@ -11239,6 +11251,12 @@
       <c r="B360">
         <v>1</v>
       </c>
+      <c r="D360">
+        <v>-0.64393199999999995</v>
+      </c>
+      <c r="E360">
+        <v>16.296029000000001</v>
+      </c>
       <c r="F360" s="1" t="s">
         <v>115</v>
       </c>
@@ -11259,6 +11277,12 @@
       <c r="B361">
         <v>2</v>
       </c>
+      <c r="D361">
+        <v>3.5703939999999998</v>
+      </c>
+      <c r="E361">
+        <v>27.157672999999999</v>
+      </c>
       <c r="F361" s="1" t="s">
         <v>137</v>
       </c>
@@ -11279,6 +11303,12 @@
       <c r="B362">
         <v>1</v>
       </c>
+      <c r="D362">
+        <v>-0.64393199999999995</v>
+      </c>
+      <c r="E362">
+        <v>16.296029000000001</v>
+      </c>
       <c r="F362" s="1" t="s">
         <v>115</v>
       </c>
@@ -11299,6 +11329,12 @@
       <c r="B363">
         <v>2</v>
       </c>
+      <c r="D363">
+        <v>-3.6909329999999998</v>
+      </c>
+      <c r="E363">
+        <v>15.260691</v>
+      </c>
       <c r="F363" s="1" t="s">
         <v>138</v>
       </c>
@@ -11319,6 +11355,12 @@
       <c r="B364">
         <v>1</v>
       </c>
+      <c r="D364">
+        <v>-3.6909329999999998</v>
+      </c>
+      <c r="E364">
+        <v>15.260691</v>
+      </c>
       <c r="F364" s="1" t="s">
         <v>138</v>
       </c>
@@ -11339,6 +11381,12 @@
       <c r="B365">
         <v>2</v>
       </c>
+      <c r="D365">
+        <v>-0.92627000000000004</v>
+      </c>
+      <c r="E365">
+        <v>10.931093000000001</v>
+      </c>
       <c r="F365" s="1" t="s">
         <v>139</v>
       </c>
@@ -11359,6 +11407,12 @@
       <c r="B366">
         <v>1</v>
       </c>
+      <c r="D366">
+        <v>-3.6909329999999998</v>
+      </c>
+      <c r="E366">
+        <v>15.260691</v>
+      </c>
       <c r="F366" s="1" t="s">
         <v>138</v>
       </c>
@@ -11379,6 +11433,12 @@
       <c r="B367">
         <v>2</v>
       </c>
+      <c r="D367">
+        <v>-5.2298070000000001</v>
+      </c>
+      <c r="E367">
+        <v>14.921853</v>
+      </c>
       <c r="F367" s="1" t="s">
         <v>111</v>
       </c>
@@ -11399,6 +11459,12 @@
       <c r="B368">
         <v>1</v>
       </c>
+      <c r="D368">
+        <v>-3.6909329999999998</v>
+      </c>
+      <c r="E368">
+        <v>15.260691</v>
+      </c>
       <c r="F368" s="1" t="s">
         <v>138</v>
       </c>
@@ -11419,6 +11485,12 @@
       <c r="B369">
         <v>2</v>
       </c>
+      <c r="D369">
+        <v>-7.101267</v>
+      </c>
+      <c r="E369">
+        <v>14.714784999999999</v>
+      </c>
       <c r="F369" s="1" t="s">
         <v>110</v>
       </c>
@@ -11439,6 +11511,12 @@
       <c r="B370">
         <v>1</v>
       </c>
+      <c r="D370">
+        <v>-5.2298070000000001</v>
+      </c>
+      <c r="E370">
+        <v>14.921853</v>
+      </c>
       <c r="F370" s="1" t="s">
         <v>111</v>
       </c>
@@ -11459,6 +11537,12 @@
       <c r="B371">
         <v>2</v>
       </c>
+      <c r="D371">
+        <v>-10.486506</v>
+      </c>
+      <c r="E371">
+        <v>20.945640999999998</v>
+      </c>
       <c r="F371" s="1" t="s">
         <v>112</v>
       </c>
@@ -11479,6 +11563,12 @@
       <c r="B372">
         <v>1</v>
       </c>
+      <c r="D372">
+        <v>-10.486506</v>
+      </c>
+      <c r="E372">
+        <v>20.945640999999998</v>
+      </c>
       <c r="F372" s="1" t="s">
         <v>112</v>
       </c>
@@ -11499,6 +11589,12 @@
       <c r="B373">
         <v>2</v>
       </c>
+      <c r="D373">
+        <v>-28.559771000000001</v>
+      </c>
+      <c r="E373">
+        <v>28.96481</v>
+      </c>
       <c r="F373" s="1" t="s">
         <v>113</v>
       </c>
@@ -11519,6 +11615,12 @@
       <c r="B374">
         <v>1</v>
       </c>
+      <c r="D374">
+        <v>-10.486506</v>
+      </c>
+      <c r="E374">
+        <v>20.945640999999998</v>
+      </c>
       <c r="F374" s="1" t="s">
         <v>112</v>
       </c>
@@ -11539,6 +11641,12 @@
       <c r="B375">
         <v>2</v>
       </c>
+      <c r="D375">
+        <v>-11.336762</v>
+      </c>
+      <c r="E375">
+        <v>22.639831999999998</v>
+      </c>
       <c r="F375" s="1" t="s">
         <v>140</v>
       </c>
@@ -11559,6 +11667,12 @@
       <c r="B376">
         <v>1</v>
       </c>
+      <c r="D376">
+        <v>-11.336762</v>
+      </c>
+      <c r="E376">
+        <v>22.639831999999998</v>
+      </c>
       <c r="F376" s="1" t="s">
         <v>140</v>
       </c>
@@ -11579,6 +11693,12 @@
       <c r="B377">
         <v>2</v>
       </c>
+      <c r="D377">
+        <v>-13.26783</v>
+      </c>
+      <c r="E377">
+        <v>33.972084000000002</v>
+      </c>
       <c r="F377" s="1" t="s">
         <v>142</v>
       </c>
@@ -11599,6 +11719,12 @@
       <c r="B378">
         <v>1</v>
       </c>
+      <c r="D378">
+        <v>-11.336762</v>
+      </c>
+      <c r="E378">
+        <v>22.639831999999998</v>
+      </c>
       <c r="F378" s="1" t="s">
         <v>140</v>
       </c>
@@ -11619,6 +11745,12 @@
       <c r="B379">
         <v>2</v>
       </c>
+      <c r="D379">
+        <v>-7.2880279999999997</v>
+      </c>
+      <c r="E379">
+        <v>26.159983</v>
+      </c>
       <c r="F379" s="1" t="s">
         <v>143</v>
       </c>
@@ -11639,6 +11771,12 @@
       <c r="B380">
         <v>1</v>
       </c>
+      <c r="D380">
+        <v>-7.2880279999999997</v>
+      </c>
+      <c r="E380">
+        <v>26.159983</v>
+      </c>
       <c r="F380" s="1" t="s">
         <v>143</v>
       </c>
@@ -11659,6 +11797,12 @@
       <c r="B381">
         <v>2</v>
       </c>
+      <c r="D381">
+        <v>-2.2998690000000002</v>
+      </c>
+      <c r="E381">
+        <v>27.007078</v>
+      </c>
       <c r="F381" s="1" t="s">
         <v>119</v>
       </c>
@@ -11679,6 +11823,12 @@
       <c r="B382">
         <v>1</v>
       </c>
+      <c r="D382">
+        <v>-7.2880279999999997</v>
+      </c>
+      <c r="E382">
+        <v>26.159983</v>
+      </c>
       <c r="F382" s="1" t="s">
         <v>143</v>
       </c>
@@ -11699,6 +11849,12 @@
       <c r="B383">
         <v>2</v>
       </c>
+      <c r="D383">
+        <v>-9.3739860000000004</v>
+      </c>
+      <c r="E383">
+        <v>29.642486000000002</v>
+      </c>
       <c r="F383" s="1" t="s">
         <v>144</v>
       </c>
@@ -11719,6 +11875,12 @@
       <c r="B384">
         <v>1</v>
       </c>
+      <c r="D384">
+        <v>-9.3739860000000004</v>
+      </c>
+      <c r="E384">
+        <v>29.642486000000002</v>
+      </c>
       <c r="F384" s="1" t="s">
         <v>144</v>
       </c>
@@ -11739,6 +11901,12 @@
       <c r="B385">
         <v>2</v>
       </c>
+      <c r="D385">
+        <v>-14.492207000000001</v>
+      </c>
+      <c r="E385">
+        <v>15.110096</v>
+      </c>
       <c r="F385" s="1" t="s">
         <v>145</v>
       </c>
@@ -11759,6 +11927,12 @@
       <c r="B386">
         <v>1</v>
       </c>
+      <c r="D386">
+        <v>-9.3739860000000004</v>
+      </c>
+      <c r="E386">
+        <v>29.642486000000002</v>
+      </c>
       <c r="F386" s="1" t="s">
         <v>144</v>
       </c>
@@ -11779,6 +11953,12 @@
       <c r="B387">
         <v>2</v>
       </c>
+      <c r="D387">
+        <v>-10.171678999999999</v>
+      </c>
+      <c r="E387">
+        <v>30.282513000000002</v>
+      </c>
       <c r="F387" s="1" t="s">
         <v>146</v>
       </c>
@@ -11794,10 +11974,16 @@
     </row>
     <row r="388" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="B388">
         <v>1</v>
+      </c>
+      <c r="D388">
+        <v>-10.171678999999999</v>
+      </c>
+      <c r="E388">
+        <v>30.282513000000002</v>
       </c>
       <c r="F388" s="1" t="s">
         <v>146</v>
@@ -11814,13 +12000,19 @@
     </row>
     <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="B389">
         <v>2</v>
       </c>
+      <c r="D389">
+        <v>-0.22980900000000001</v>
+      </c>
+      <c r="E389">
+        <v>30.903717</v>
+      </c>
       <c r="F389" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H389" t="s">
         <v>88</v>
@@ -11834,13 +12026,19 @@
     </row>
     <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B390">
         <v>1</v>
       </c>
+      <c r="D390">
+        <v>-10.171678999999999</v>
+      </c>
+      <c r="E390">
+        <v>30.282513000000002</v>
+      </c>
       <c r="F390" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H390" t="s">
         <v>88</v>
@@ -11854,13 +12052,19 @@
     </row>
     <row r="391" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B391">
         <v>2</v>
       </c>
+      <c r="D391">
+        <v>-10.708545000000001</v>
+      </c>
+      <c r="E391">
+        <v>30.677824000000001</v>
+      </c>
       <c r="F391" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H391" t="s">
         <v>88</v>
@@ -11874,10 +12078,16 @@
     </row>
     <row r="392" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B392">
         <v>1</v>
+      </c>
+      <c r="D392">
+        <v>-10.708545000000001</v>
+      </c>
+      <c r="E392">
+        <v>30.677824000000001</v>
       </c>
       <c r="F392" s="1" t="s">
         <v>149</v>
@@ -11894,13 +12104,19 @@
     </row>
     <row r="393" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B393">
         <v>2</v>
       </c>
+      <c r="D393">
+        <v>-11.871508</v>
+      </c>
+      <c r="E393">
+        <v>31.242554999999999</v>
+      </c>
       <c r="F393" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H393" t="s">
         <v>88</v>
@@ -11914,13 +12130,19 @@
     </row>
     <row r="394" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="B394">
         <v>1</v>
       </c>
+      <c r="D394">
+        <v>-10.708545000000001</v>
+      </c>
+      <c r="E394">
+        <v>30.677824000000001</v>
+      </c>
       <c r="F394" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H394" t="s">
         <v>88</v>
@@ -11934,13 +12156,19 @@
     </row>
     <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="B395">
         <v>2</v>
       </c>
+      <c r="D395">
+        <v>-3.841202</v>
+      </c>
+      <c r="E395">
+        <v>33.727367000000001</v>
+      </c>
       <c r="F395" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H395" t="s">
         <v>88</v>
@@ -11954,10 +12182,16 @@
     </row>
     <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B396">
         <v>1</v>
+      </c>
+      <c r="D396">
+        <v>-3.841202</v>
+      </c>
+      <c r="E396">
+        <v>33.727367000000001</v>
       </c>
       <c r="F396" s="1" t="s">
         <v>150</v>
@@ -11974,13 +12208,19 @@
     </row>
     <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B397">
         <v>2</v>
       </c>
+      <c r="D397">
+        <v>-1.7354909999999999</v>
+      </c>
+      <c r="E397">
+        <v>29.378945000000002</v>
+      </c>
       <c r="F397" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="H397" t="s">
         <v>88</v>
@@ -11994,13 +12234,19 @@
     </row>
     <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="B398">
         <v>1</v>
       </c>
+      <c r="D398">
+        <v>-3.841202</v>
+      </c>
+      <c r="E398">
+        <v>33.727367000000001</v>
+      </c>
       <c r="F398" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="H398" t="s">
         <v>88</v>
@@ -12014,13 +12260,19 @@
     </row>
     <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="B399">
         <v>2</v>
       </c>
+      <c r="D399">
+        <v>-1.453236</v>
+      </c>
+      <c r="E399">
+        <v>36.080410000000001</v>
+      </c>
       <c r="F399" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="H399" t="s">
         <v>88</v>
@@ -12034,13 +12286,19 @@
     </row>
     <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B400">
         <v>1</v>
       </c>
+      <c r="D400">
+        <v>-1.453236</v>
+      </c>
+      <c r="E400">
+        <v>36.080410000000001</v>
+      </c>
       <c r="F400" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="H400" t="s">
         <v>88</v>
@@ -12054,13 +12312,19 @@
     </row>
     <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B401">
         <v>2</v>
       </c>
+      <c r="D401">
+        <v>-1.4155990000000001</v>
+      </c>
+      <c r="E401">
+        <v>38.376978999999999</v>
+      </c>
       <c r="F401" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H401" t="s">
         <v>88</v>
@@ -12069,6 +12333,58 @@
         <v>76</v>
       </c>
       <c r="J401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A402" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B402">
+        <v>1</v>
+      </c>
+      <c r="D402">
+        <v>-1.4155990000000001</v>
+      </c>
+      <c r="E402">
+        <v>38.376978999999999</v>
+      </c>
+      <c r="F402" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H402" t="s">
+        <v>88</v>
+      </c>
+      <c r="I402" t="s">
+        <v>76</v>
+      </c>
+      <c r="J402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A403" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B403">
+        <v>2</v>
+      </c>
+      <c r="D403">
+        <v>-4.5733680000000003</v>
+      </c>
+      <c r="E403">
+        <v>37.868721999999998</v>
+      </c>
+      <c r="F403" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H403" t="s">
+        <v>88</v>
+      </c>
+      <c r="I403" t="s">
+        <v>76</v>
+      </c>
+      <c r="J403">
         <v>1</v>
       </c>
     </row>

</xml_diff>